<commit_message>
aggiornamento 2026 02 04 12:49
</commit_message>
<xml_diff>
--- a/networking/verfica/tabella indirizzi ip.xlsx
+++ b/networking/verfica/tabella indirizzi ip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RickyMandich\PROJECT\appuntiITS\networking\verfica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF03973-775E-43C0-B75F-856D72542A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350FCF78-DD9E-4169-8F43-ECD66FBFE99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{294B2727-FDEC-4C09-AD72-7998F5E81237}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -179,11 +179,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9B0A49-D915-4162-B15D-BE1027FEE134}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
@@ -578,21 +578,21 @@
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2152,236 +2152,236 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="10">
-        <v>192</v>
-      </c>
-      <c r="D45" s="10">
-        <v>168</v>
-      </c>
-      <c r="E45" s="10">
-        <v>1</v>
-      </c>
-      <c r="F45" s="10">
+      <c r="C45" s="9">
+        <v>192</v>
+      </c>
+      <c r="D45" s="9">
+        <v>168</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1</v>
+      </c>
+      <c r="F45" s="9">
         <v>96</v>
       </c>
-      <c r="G45" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" s="10">
-        <v>192</v>
-      </c>
-      <c r="I45" s="10">
-        <v>168</v>
-      </c>
-      <c r="J45" s="10">
-        <v>1</v>
-      </c>
-      <c r="K45" s="10">
+      <c r="G45" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="9">
+        <v>192</v>
+      </c>
+      <c r="I45" s="9">
+        <v>168</v>
+      </c>
+      <c r="J45" s="9">
+        <v>1</v>
+      </c>
+      <c r="K45" s="9">
         <f>F45+1</f>
         <v>97</v>
       </c>
-      <c r="L45" s="11" t="s">
+      <c r="L45" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="10" t="s">
+      <c r="A46" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="10">
-        <v>192</v>
-      </c>
-      <c r="D46" s="10">
-        <v>168</v>
-      </c>
-      <c r="E46" s="10">
-        <v>1</v>
-      </c>
-      <c r="F46" s="10">
+      <c r="C46" s="9">
+        <v>192</v>
+      </c>
+      <c r="D46" s="9">
+        <v>168</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
+      <c r="F46" s="9">
         <v>96</v>
       </c>
-      <c r="G46" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="10">
-        <v>192</v>
-      </c>
-      <c r="I46" s="10">
-        <v>168</v>
-      </c>
-      <c r="J46" s="10">
-        <v>1</v>
-      </c>
-      <c r="K46" s="10">
+      <c r="G46" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="9">
+        <v>192</v>
+      </c>
+      <c r="I46" s="9">
+        <v>168</v>
+      </c>
+      <c r="J46" s="9">
+        <v>1</v>
+      </c>
+      <c r="K46" s="9">
         <f>K45+1</f>
         <v>98</v>
       </c>
-      <c r="L46" s="11" t="s">
+      <c r="L46" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="10">
-        <v>192</v>
-      </c>
-      <c r="D47" s="10">
-        <v>168</v>
-      </c>
-      <c r="E47" s="10">
-        <v>1</v>
-      </c>
-      <c r="F47" s="10">
+      <c r="C47" s="9">
+        <v>192</v>
+      </c>
+      <c r="D47" s="9">
+        <v>168</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="F47" s="9">
         <v>100</v>
       </c>
-      <c r="G47" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H47" s="10">
-        <v>192</v>
-      </c>
-      <c r="I47" s="10">
-        <v>168</v>
-      </c>
-      <c r="J47" s="10">
-        <v>1</v>
-      </c>
-      <c r="K47" s="10">
+      <c r="G47" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="9">
+        <v>192</v>
+      </c>
+      <c r="I47" s="9">
+        <v>168</v>
+      </c>
+      <c r="J47" s="9">
+        <v>1</v>
+      </c>
+      <c r="K47" s="9">
         <f>F47+1</f>
         <v>101</v>
       </c>
-      <c r="L47" s="11" t="s">
+      <c r="L47" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" s="10" t="s">
+      <c r="A48" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="10">
-        <v>192</v>
-      </c>
-      <c r="D48" s="10">
-        <v>168</v>
-      </c>
-      <c r="E48" s="10">
-        <v>1</v>
-      </c>
-      <c r="F48" s="10">
+      <c r="C48" s="9">
+        <v>192</v>
+      </c>
+      <c r="D48" s="9">
+        <v>168</v>
+      </c>
+      <c r="E48" s="9">
+        <v>1</v>
+      </c>
+      <c r="F48" s="9">
         <v>100</v>
       </c>
-      <c r="G48" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" s="10">
-        <v>192</v>
-      </c>
-      <c r="I48" s="10">
-        <v>168</v>
-      </c>
-      <c r="J48" s="10">
-        <v>1</v>
-      </c>
-      <c r="K48" s="10">
-        <f t="shared" ref="K47:K50" si="1">K47+1</f>
+      <c r="G48" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="9">
+        <v>192</v>
+      </c>
+      <c r="I48" s="9">
+        <v>168</v>
+      </c>
+      <c r="J48" s="9">
+        <v>1</v>
+      </c>
+      <c r="K48" s="9">
+        <f>K47+1</f>
         <v>102</v>
       </c>
-      <c r="L48" s="11" t="s">
+      <c r="L48" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="10">
-        <v>192</v>
-      </c>
-      <c r="D49" s="10">
-        <v>168</v>
-      </c>
-      <c r="E49" s="10">
-        <v>1</v>
-      </c>
-      <c r="F49" s="10">
+      <c r="C49" s="9">
+        <v>192</v>
+      </c>
+      <c r="D49" s="9">
+        <v>168</v>
+      </c>
+      <c r="E49" s="9">
+        <v>1</v>
+      </c>
+      <c r="F49" s="9">
         <v>104</v>
       </c>
-      <c r="G49" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H49" s="10">
-        <v>192</v>
-      </c>
-      <c r="I49" s="10">
-        <v>168</v>
-      </c>
-      <c r="J49" s="10">
-        <v>1</v>
-      </c>
-      <c r="K49" s="10">
+      <c r="G49" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="9">
+        <v>192</v>
+      </c>
+      <c r="I49" s="9">
+        <v>168</v>
+      </c>
+      <c r="J49" s="9">
+        <v>1</v>
+      </c>
+      <c r="K49" s="9">
         <f>F49+1</f>
         <v>105</v>
       </c>
-      <c r="L49" s="11" t="s">
+      <c r="L49" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="10" t="s">
+      <c r="A50" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="10">
-        <v>192</v>
-      </c>
-      <c r="D50" s="10">
-        <v>168</v>
-      </c>
-      <c r="E50" s="10">
-        <v>1</v>
-      </c>
-      <c r="F50" s="10">
+      <c r="C50" s="9">
+        <v>192</v>
+      </c>
+      <c r="D50" s="9">
+        <v>168</v>
+      </c>
+      <c r="E50" s="9">
+        <v>1</v>
+      </c>
+      <c r="F50" s="9">
         <v>104</v>
       </c>
-      <c r="G50" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="10">
-        <v>192</v>
-      </c>
-      <c r="I50" s="10">
-        <v>168</v>
-      </c>
-      <c r="J50" s="10">
-        <v>1</v>
-      </c>
-      <c r="K50" s="10">
-        <f t="shared" si="1"/>
+      <c r="G50" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="9">
+        <v>192</v>
+      </c>
+      <c r="I50" s="9">
+        <v>168</v>
+      </c>
+      <c r="J50" s="9">
+        <v>1</v>
+      </c>
+      <c r="K50" s="9">
+        <f t="shared" ref="K50" si="1">K49+1</f>
         <v>106</v>
       </c>
-      <c r="L50" s="11" t="s">
+      <c r="L50" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2391,7 +2391,8 @@
     <mergeCell ref="C4:F4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>